<commit_message>
get disease classification & update clustering model
</commit_message>
<xml_diff>
--- a/static/files/rm/klasifikasi.xlsx
+++ b/static/files/rm/klasifikasi.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dokumen Kuliah\Skripsi Binus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DD574196-B054-41D7-B6A4-31A4FE51E9DE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5BA9911-EFA2-439F-8C53-A9BB1A801629}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2FDAE665-CE98-4688-9059-D2FF564BC64E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
   <si>
     <t>bab</t>
   </si>
@@ -54,31 +54,212 @@
     <t>III</t>
   </si>
   <si>
-    <t>A01-A99</t>
-  </si>
-  <si>
-    <t>B01-B99</t>
-  </si>
-  <si>
-    <t>C01-C99</t>
-  </si>
-  <si>
-    <t>AA</t>
-  </si>
-  <si>
-    <t>BB</t>
-  </si>
-  <si>
-    <t>CC</t>
+    <t>IV</t>
+  </si>
+  <si>
+    <t>VI</t>
+  </si>
+  <si>
+    <t>VII</t>
+  </si>
+  <si>
+    <t>VIII</t>
+  </si>
+  <si>
+    <t>IX</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>XI</t>
+  </si>
+  <si>
+    <t>XII</t>
+  </si>
+  <si>
+    <t>XIII</t>
+  </si>
+  <si>
+    <t>XIV</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>XV</t>
+  </si>
+  <si>
+    <t>XVI</t>
+  </si>
+  <si>
+    <t>XVII</t>
+  </si>
+  <si>
+    <t>XVIII</t>
+  </si>
+  <si>
+    <t>XIX</t>
+  </si>
+  <si>
+    <t>XX</t>
+  </si>
+  <si>
+    <t>XXI</t>
+  </si>
+  <si>
+    <t>XXII</t>
+  </si>
+  <si>
+    <t>A00-B99</t>
+  </si>
+  <si>
+    <t>C00-D48</t>
+  </si>
+  <si>
+    <t>D50-D89</t>
+  </si>
+  <si>
+    <t>E00-E90</t>
+  </si>
+  <si>
+    <t>F00-F99</t>
+  </si>
+  <si>
+    <t>G00-G99</t>
+  </si>
+  <si>
+    <t>H00-H59</t>
+  </si>
+  <si>
+    <t>H60-H95</t>
+  </si>
+  <si>
+    <t>I00-I99</t>
+  </si>
+  <si>
+    <t>J00-J99</t>
+  </si>
+  <si>
+    <t>K00-K93</t>
+  </si>
+  <si>
+    <t>L00-L99</t>
+  </si>
+  <si>
+    <t>M00-M99</t>
+  </si>
+  <si>
+    <t>N00-N99</t>
+  </si>
+  <si>
+    <t>O00-O99</t>
+  </si>
+  <si>
+    <t>P00-P96</t>
+  </si>
+  <si>
+    <t>Q00-Q99</t>
+  </si>
+  <si>
+    <t>R00-R99</t>
+  </si>
+  <si>
+    <t>S00-T98</t>
+  </si>
+  <si>
+    <t>V01-Y98</t>
+  </si>
+  <si>
+    <t>Z00-Z99</t>
+  </si>
+  <si>
+    <t>U00-U99</t>
+  </si>
+  <si>
+    <t>Penyakit Infeksi dan parasit</t>
+  </si>
+  <si>
+    <t>Neoplasma</t>
+  </si>
+  <si>
+    <t>Penyakit darah dan organ pembentuk darah termasuk ganguan sistem
+imun</t>
+  </si>
+  <si>
+    <t>Endokrin, nutrisi dan ganguan metabolik</t>
+  </si>
+  <si>
+    <t>Penyakit yg mengenai sistem syaraf</t>
+  </si>
+  <si>
+    <t>Penyakit mata dan adnexa</t>
+  </si>
+  <si>
+    <t>Penyakit telinga dan mastoid</t>
+  </si>
+  <si>
+    <t>Penyakit pada sistem sirkulasi</t>
+  </si>
+  <si>
+    <t>Penyakit pada sistem pernafasan</t>
+  </si>
+  <si>
+    <t>Penyakit pada sistem pencernaan</t>
+  </si>
+  <si>
+    <t>Penyakit pada kulit dan jaringan subcutaneous</t>
+  </si>
+  <si>
+    <t>Penyakit pada sistem musculoskletal</t>
+  </si>
+  <si>
+    <t>Penyakit pada sistem saluran kemih dan genital</t>
+  </si>
+  <si>
+    <t>Kehamilan dan kelahiran</t>
+  </si>
+  <si>
+    <t>Keadaan yg berasal dari periode perinatal</t>
+  </si>
+  <si>
+    <t>Malformasi kongenital, deformasi dan kelainan chromosom</t>
+  </si>
+  <si>
+    <t>Gejala, tanda, kelainan klinik dan kelainan lab yg tidak ditemukan pada
+klasifikasi lain</t>
+  </si>
+  <si>
+    <t>Keracunan, cedera dan beberapa penyebab yg dari luar</t>
+  </si>
+  <si>
+    <t>Penyebab morbiditas dan kematian eksternal</t>
+  </si>
+  <si>
+    <t>Faktor faktor yg memengaruhi status kesehatan dan hubungannya
+dengan jasa kesehatan</t>
+  </si>
+  <si>
+    <t>Kode kegunaan khusus</t>
+  </si>
+  <si>
+    <t>Gangguan jiwa dan prilaku</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -105,8 +286,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -421,13 +606,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8B3D35F-3E94-43F0-8DD9-E9D248E696F5}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="57" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -445,10 +633,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -456,24 +644,234 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>